<commit_message>
fixed error with loading info from source file into db
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\pipenv\TimeManagment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83710557-A0FB-4A65-8E20-799EC9392FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85D6D21-4B34-4F6B-BF75-DE2AA01E39FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B9F310CC-F0E0-405B-8717-4BEB3E80AF7B}"/>
   </bookViews>
@@ -1279,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD59C1A2-92B6-4584-ADD1-BEC4F87CA089}">
   <dimension ref="A1:D170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1313,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>39</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>39</v>
@@ -1985,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>39</v>
@@ -2321,7 +2321,7 @@
         <v>3</v>
       </c>
       <c r="C74" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>39</v>
@@ -2657,7 +2657,7 @@
         <v>4</v>
       </c>
       <c r="C98" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>39</v>
@@ -2993,7 +2993,7 @@
         <v>5</v>
       </c>
       <c r="C122" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>39</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="B125">
         <v>5</v>
@@ -3329,7 +3329,7 @@
         <v>6</v>
       </c>
       <c r="C146" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>39</v>

</xml_diff>